<commit_message>
more work on parameter testing
</commit_message>
<xml_diff>
--- a/th_UNet rewrites/trainingCombinationDetails.xlsx
+++ b/th_UNet rewrites/trainingCombinationDetails.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theophanemayaud/Dev/EPFL MA1/Machine Learning/cs-433-project-2-ml_fools/th_UNet rewrites/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE2AB49-278F-5B45-BF15-8A3FAA688D6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C37AC5C5-223C-E443-9562-C3D89403546A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="11300" windowWidth="28800" windowHeight="17500" xr2:uid="{06BBF387-671E-BD4A-8DD6-D75923AA206F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{06BBF387-671E-BD4A-8DD6-D75923AA206F}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="39">
   <si>
     <t>train images</t>
   </si>
@@ -79,19 +79,97 @@
   </si>
   <si>
     <t>one big outlier negative, but overall it really underestimates</t>
+  </si>
+  <si>
+    <t>SGD no inertia</t>
+  </si>
+  <si>
+    <t>30 first of dataset</t>
+  </si>
+  <si>
+    <t>30 from 300 to 330</t>
+  </si>
+  <si>
+    <t>thousands of percent negative</t>
+  </si>
+  <si>
+    <t>very negative…</t>
+  </si>
+  <si>
+    <t>training notes</t>
+  </si>
+  <si>
+    <t>loss seemed to go down fast and then be around 0.1, reducing every time. But results seem all zero, so very bad !</t>
+  </si>
+  <si>
+    <t>results look ok ish, with a lot of bark</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Loss diverges almost immediately</t>
+  </si>
+  <si>
+    <t>SGD inertia 0.9</t>
+  </si>
+  <si>
+    <t>Loss goes down very fast and then very slowly but is around 0.2 Results are all black though on training and testing images</t>
+  </si>
+  <si>
+    <t>Seems all black…</t>
+  </si>
+  <si>
+    <t>2 first of dataset</t>
+  </si>
+  <si>
+    <t>all predictions seem all black although loss goes from very high thousands to under 1 very quickly, and then slighly moves lower and lower…</t>
+  </si>
+  <si>
+    <t>all seem black</t>
+  </si>
+  <si>
+    <t>all seem black…</t>
+  </si>
+  <si>
+    <t>printing all images during training as lr=1e-4 abd 1e-5 were all black… Now not all seem black !</t>
+  </si>
+  <si>
+    <t>while training, losses go down slowly and are like 0.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">way under estimated, but still a few values above and near 0 </t>
+  </si>
+  <si>
+    <t>Between -1'000% and 0% or a little above, doesn't look too bad</t>
+  </si>
+  <si>
+    <t>very clearly embolism regions selected, but a lot of bark and some surrounding.</t>
+  </si>
+  <si>
+    <t>a lot of other stuff predicted : bark, surrounding, but still looks not terrible. All values overestimate, from 100% to 10000%. Mostly under 3500% though</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF212121"/>
+      <name val="Courier New"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -120,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -134,6 +212,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,11 +528,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{321E1C99-B8DB-8C43-AF4F-C138A0210910}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -461,17 +541,18 @@
     <col min="2" max="2" width="9.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" style="1"/>
-    <col min="8" max="8" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.83203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="10.83203125" style="1"/>
+    <col min="6" max="6" width="11" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.1640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.5" style="1" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -485,30 +566,33 @@
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="H1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="68" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>30</v>
+    <row r="2" spans="1:12" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B2" s="1">
         <v>30</v>
@@ -519,27 +603,302 @@
       <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="2">
         <v>1E-4</v>
       </c>
-      <c r="F2" s="1">
-        <v>20</v>
-      </c>
-      <c r="G2" s="1">
+      <c r="G2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="3">
+        <v>-9.4968849730083793</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="3">
+        <v>-0.47441138720441201</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="86" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1">
         <v>30</v>
       </c>
-      <c r="H2" s="3">
-        <v>-9.4968849730083793</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="3">
-        <v>-0.47441138720441201</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="6">
+        <v>-8552.9666666666599</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="6">
+        <v>-44497.4</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="35" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="52" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1">
+        <v>30</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="G5" s="5">
+        <v>43</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="6">
+        <v>-12.750031099293899</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" s="6">
+        <v>-3.01474602378961</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="35" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" s="1">
+        <v>500</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="I6" s="6"/>
+      <c r="K6" s="6"/>
+    </row>
+    <row r="7" spans="1:12" ht="19" x14ac:dyDescent="0.25">
+      <c r="F7" s="2"/>
+      <c r="G7" s="5"/>
+      <c r="I7" s="6"/>
+      <c r="K7" s="6"/>
+    </row>
+    <row r="8" spans="1:12" ht="86" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="6">
+        <v>-8552.9666666666599</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K8" s="6">
+        <v>-44497.4</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="86" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="1">
+        <v>100</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" s="6">
+        <v>-8552.9666666666599</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K9" s="6">
+        <v>-31249.5</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="137" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="1">
+        <v>100</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="2">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" s="6">
+        <v>11.7450188966778</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K10" s="6">
+        <v>0.91483316935589598</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="52" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1">
+        <v>30</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="2">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="K11" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>